<commit_message>
J'ai rempli ma Parti pour ce Lundi 17/02/2014
Il ne me reste qu'un petit soucis, celui de l'aperçu des photos !
</commit_message>
<xml_diff>
--- a/Daily Meetings.xlsx
+++ b/Daily Meetings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khalil\Documents\GitHub\Daily_Meentings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\GitHub\Daily_Meentings\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="56">
   <si>
     <t>Mardi 11-02-2014</t>
   </si>
@@ -183,6 +183,15 @@
   </si>
   <si>
     <t>CRUDE Commentaires -  JAVA Web Application</t>
+  </si>
+  <si>
+    <t>Lundi 17-02-2014</t>
+  </si>
+  <si>
+    <t>Comment avoir un aperçu de la photo après Upload.</t>
+  </si>
+  <si>
+    <t>Ajout + Modification + Suppression + Affichage + Upload des Photos dans Base de Données</t>
   </si>
 </sst>
 </file>
@@ -391,7 +400,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -415,6 +424,75 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -424,54 +502,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -481,23 +511,20 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -517,23 +544,8 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -820,10 +832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33:M33"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41:J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,54 +848,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
@@ -930,710 +942,908 @@
     <row r="7" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18"/>
       <c r="B7" s="18"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
     </row>
     <row r="8" spans="1:13" ht="27.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="36"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="28" t="s">
+      <c r="F8" s="27"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="29"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="12" t="s">
+      <c r="I8" s="36"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="L8" s="12"/>
-      <c r="M8" s="13"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="10"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
-      <c r="B9" s="36"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="15"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="14"/>
     </row>
     <row r="10" spans="1:13" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
-      <c r="B10" s="36"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="32" t="s">
+      <c r="E10" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="21"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="I10" s="33"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="16" t="s">
+      <c r="I10" s="30"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="L10" s="16"/>
-      <c r="M10" s="17"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="12"/>
     </row>
     <row r="11" spans="1:13" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
-      <c r="B11" s="36"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="32" t="s">
+      <c r="F11" s="27"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="33"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="16" t="s">
+      <c r="I11" s="30"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="16"/>
-      <c r="M11" s="17"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="12"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
-      <c r="B12" s="36"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="15"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="14"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="36"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="23"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I13" s="10"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="L13" s="14"/>
-      <c r="M13" s="15"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="33"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="L13" s="13"/>
+      <c r="M13" s="14"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="36"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="15"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="14"/>
     </row>
     <row r="15" spans="1:13" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
-      <c r="B15" s="36"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="20"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="29"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L15" s="12"/>
-      <c r="M15" s="13"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="36"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L15" s="9"/>
+      <c r="M15" s="10"/>
     </row>
     <row r="16" spans="1:13" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
-      <c r="B16" s="36"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="20"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L16" s="12"/>
-      <c r="M16" s="13"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="36"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16" s="9"/>
+      <c r="M16" s="10"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
-      <c r="B17" s="36"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="17"/>
       <c r="C17" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="22"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="15"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="14"/>
     </row>
     <row r="18" spans="1:13" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="36"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="26"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="32" t="s">
+      <c r="E18" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="21"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="I18" s="33"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="16" t="s">
+      <c r="I18" s="30"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="L18" s="16"/>
-      <c r="M18" s="17"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="12"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="22"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="15"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="14"/>
     </row>
     <row r="20" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
-      <c r="B20" s="36"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" s="26"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="32" t="s">
+      <c r="E20" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="21"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="I20" s="33"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L20" s="12"/>
-      <c r="M20" s="13"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" s="9"/>
+      <c r="M20" s="10"/>
     </row>
     <row r="21" spans="1:13" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
-      <c r="B21" s="36"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="17"/>
       <c r="C21" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="38"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="40" t="s">
+      <c r="E21" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="44"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="I21" s="41"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="43" t="s">
+      <c r="I21" s="47"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="L21" s="43"/>
-      <c r="M21" s="44"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="39"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
-      <c r="B22" s="36"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="17"/>
       <c r="C22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="22"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="15"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="14"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="36"/>
+      <c r="B23" s="17"/>
       <c r="C23" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="22" t="s">
+      <c r="E23" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="F23" s="23"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I23" s="10"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="L23" s="14"/>
-      <c r="M23" s="15"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="33"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="L23" s="13"/>
+      <c r="M23" s="14"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
-      <c r="B24" s="36"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="17"/>
       <c r="C24" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="22"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="15"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="14"/>
     </row>
     <row r="25" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
-      <c r="B25" s="36"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="45" t="s">
+      <c r="E25" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="46"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="32" t="s">
+      <c r="F25" s="41"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="I25" s="33"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L25" s="12"/>
-      <c r="M25" s="13"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L25" s="9"/>
+      <c r="M25" s="10"/>
     </row>
     <row r="26" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
-      <c r="B26" s="36"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="17"/>
       <c r="C26" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="25" t="s">
+      <c r="E26" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F26" s="26"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" s="29"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L26" s="12"/>
-      <c r="M26" s="13"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" s="36"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L26" s="9"/>
+      <c r="M26" s="10"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
-      <c r="B27" s="36"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="17"/>
       <c r="C27" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E27" s="22"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="13"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="10"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="36"/>
+      <c r="B28" s="17"/>
       <c r="C28" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F28" s="23"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="9" t="s">
+      <c r="E28" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="24"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="I28" s="10"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="L28" s="14"/>
-      <c r="M28" s="15"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="L28" s="13"/>
+      <c r="M28" s="14"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
-      <c r="B29" s="36"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="22"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="15"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="14"/>
     </row>
     <row r="30" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="35"/>
-      <c r="B30" s="36"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="17"/>
       <c r="C30" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="19" t="s">
+      <c r="E30" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="F30" s="20"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="I30" s="29"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L30" s="12"/>
-      <c r="M30" s="13"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="I30" s="36"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L30" s="9"/>
+      <c r="M30" s="10"/>
     </row>
     <row r="31" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="35"/>
-      <c r="B31" s="36"/>
+      <c r="A31" s="16"/>
+      <c r="B31" s="17"/>
       <c r="C31" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E31" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="F31" s="26"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="32" t="s">
+      <c r="E31" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" s="21"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="I31" s="33"/>
-      <c r="J31" s="34"/>
-      <c r="K31" s="12" t="s">
+      <c r="I31" s="30"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="L31" s="12"/>
-      <c r="M31" s="13"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="10"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="35"/>
-      <c r="B32" s="36"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="17"/>
       <c r="C32" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E32" s="22"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="15"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="34"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="14"/>
     </row>
     <row r="33" spans="1:13" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="36"/>
+      <c r="B33" s="17"/>
       <c r="C33" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="25" t="s">
+      <c r="E33" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="F33" s="26"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="32" t="s">
+      <c r="F33" s="21"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="I33" s="33"/>
-      <c r="J33" s="34"/>
-      <c r="K33" s="12" t="s">
+      <c r="I33" s="30"/>
+      <c r="J33" s="31"/>
+      <c r="K33" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="L33" s="12"/>
-      <c r="M33" s="13"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="10"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="35"/>
-      <c r="B34" s="36"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="17"/>
       <c r="C34" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E34" s="22"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="15"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="14"/>
     </row>
     <row r="35" spans="1:13" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="35"/>
-      <c r="B35" s="36"/>
+      <c r="A35" s="16"/>
+      <c r="B35" s="17"/>
       <c r="C35" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E35" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="F35" s="26"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="I35" s="33"/>
-      <c r="J35" s="34"/>
-      <c r="K35" s="12" t="s">
+      <c r="E35" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F35" s="21"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="I35" s="30"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="L35" s="12"/>
-      <c r="M35" s="13"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="10"/>
     </row>
     <row r="36" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="35"/>
-      <c r="B36" s="36"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="17"/>
       <c r="C36" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E36" s="19" t="s">
+      <c r="E36" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="F36" s="20"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="28" t="s">
+      <c r="F36" s="27"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="I36" s="29"/>
-      <c r="J36" s="30"/>
-      <c r="K36" s="16" t="s">
+      <c r="I36" s="36"/>
+      <c r="J36" s="37"/>
+      <c r="K36" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="L36" s="16"/>
-      <c r="M36" s="17"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="12"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="35"/>
-      <c r="B37" s="36"/>
+      <c r="A37" s="16"/>
+      <c r="B37" s="17"/>
       <c r="C37" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E37" s="22"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="28"/>
-      <c r="I37" s="29"/>
-      <c r="J37" s="30"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="15"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="14"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="49"/>
+      <c r="C38" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="20"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="31"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="10"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="49"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="23"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="34"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="14"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="49"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40" s="20"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="31"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="10"/>
+    </row>
+    <row r="41" spans="1:13" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="49"/>
+      <c r="B41" s="49"/>
+      <c r="C41" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F41" s="27"/>
+      <c r="G41" s="28"/>
+      <c r="H41" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="I41" s="30"/>
+      <c r="J41" s="31"/>
+      <c r="K41" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="L41" s="11"/>
+      <c r="M41" s="12"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="49"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" s="23"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="35"/>
+      <c r="I42" s="36"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="103">
+  <mergeCells count="119">
+    <mergeCell ref="A38:B42"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:J38"/>
+    <mergeCell ref="K38:M38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="K39:M39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="K40:M40"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:J41"/>
+    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="K42:M42"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="A5:B7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="E5:G7"/>
+    <mergeCell ref="H5:J7"/>
+    <mergeCell ref="K5:M7"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="A8:B12"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="A13:B17"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="A18:B22"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="A23:B27"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="H32:J32"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
     <mergeCell ref="K35:M35"/>
     <mergeCell ref="K36:M36"/>
     <mergeCell ref="K37:M37"/>
@@ -1658,85 +1868,6 @@
     <mergeCell ref="K27:M27"/>
     <mergeCell ref="A28:B32"/>
     <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="H28:J28"/>
-    <mergeCell ref="H29:J29"/>
-    <mergeCell ref="H30:J30"/>
-    <mergeCell ref="H31:J31"/>
-    <mergeCell ref="H32:J32"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="K28:M28"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="K30:M30"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="A23:B27"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="H25:J25"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="A18:B22"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="A13:B17"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="A5:B7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="E5:G7"/>
-    <mergeCell ref="H5:J7"/>
-    <mergeCell ref="K5:M7"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="A8:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
La partie de Lundi
:*
</commit_message>
<xml_diff>
--- a/Daily Meetings.xlsx
+++ b/Daily Meetings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\GitHub\Daily_Meentings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khalil\Documents\GitHub\Daily_Meentings\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="58">
   <si>
     <t>Mardi 11-02-2014</t>
   </si>
@@ -176,12 +176,6 @@
     <t>Classe interaction base de données (DAO)</t>
   </si>
   <si>
-    <t>DAO</t>
-  </si>
-  <si>
-    <t>les requêtes SQL(modification, suppression)</t>
-  </si>
-  <si>
     <t>CRUDE Commentaires -  JAVA Web Application</t>
   </si>
   <si>
@@ -192,6 +186,18 @@
   </si>
   <si>
     <t>Ajout + Modification + Suppression + Affichage + Upload des Photos dans Base de Données</t>
+  </si>
+  <si>
+    <t>les requêtes SQL</t>
+  </si>
+  <si>
+    <t>DAO Connexion BDD</t>
+  </si>
+  <si>
+    <t>Requêtes SQL</t>
+  </si>
+  <si>
+    <t>CRUDE Commentaires</t>
   </si>
 </sst>
 </file>
@@ -424,128 +430,128 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -834,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41:J41"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38:M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,117 +854,117 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18" t="s">
+      <c r="B5" s="34"/>
+      <c r="C5" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18" t="s">
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18" t="s">
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
     </row>
     <row r="6" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
     </row>
     <row r="7" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
     </row>
     <row r="8" spans="1:13" ht="27.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="17"/>
+      <c r="B8" s="37"/>
       <c r="C8" s="3" t="s">
         <v>1</v>
       </c>
@@ -970,64 +976,64 @@
       </c>
       <c r="F8" s="27"/>
       <c r="G8" s="28"/>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="36"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="9" t="s">
+      <c r="I8" s="32"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="L8" s="9"/>
-      <c r="M8" s="10"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="17"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="17"/>
+      <c r="A9" s="36"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="14"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="25"/>
     </row>
     <row r="10" spans="1:13" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="17"/>
+      <c r="A10" s="36"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="29" t="s">
+      <c r="E10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="I10" s="30"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="11" t="s">
+      <c r="I10" s="14"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="L10" s="11"/>
-      <c r="M10" s="12"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="30"/>
     </row>
     <row r="11" spans="1:13" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="17"/>
+      <c r="A11" s="36"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="3" t="s">
         <v>4</v>
       </c>
@@ -1039,85 +1045,85 @@
       </c>
       <c r="F11" s="27"/>
       <c r="G11" s="28"/>
-      <c r="H11" s="29" t="s">
+      <c r="H11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="30"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="11" t="s">
+      <c r="I11" s="14"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="11"/>
-      <c r="M11" s="12"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="30"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="17"/>
+      <c r="A12" s="36"/>
+      <c r="B12" s="37"/>
       <c r="C12" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="23"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="14"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="25"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="17"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="I13" s="33"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L13" s="13"/>
-      <c r="M13" s="14"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="22"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="L13" s="24"/>
+      <c r="M13" s="25"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="17"/>
+      <c r="A14" s="36"/>
+      <c r="B14" s="37"/>
       <c r="C14" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="23"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="14"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="25"/>
     </row>
     <row r="15" spans="1:13" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="17"/>
+      <c r="A15" s="36"/>
+      <c r="B15" s="37"/>
       <c r="C15" s="3" t="s">
         <v>19</v>
       </c>
@@ -1129,20 +1135,20 @@
       </c>
       <c r="F15" s="27"/>
       <c r="G15" s="28"/>
-      <c r="H15" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="36"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="L15" s="9"/>
-      <c r="M15" s="10"/>
+      <c r="H15" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="32"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="L15" s="16"/>
+      <c r="M15" s="17"/>
     </row>
     <row r="16" spans="1:13" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="17"/>
+      <c r="A16" s="36"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="3" t="s">
         <v>4</v>
       </c>
@@ -1154,315 +1160,315 @@
       </c>
       <c r="F16" s="27"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="36"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="L16" s="9"/>
-      <c r="M16" s="10"/>
+      <c r="H16" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="32"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16" s="16"/>
+      <c r="M16" s="17"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="17"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="37"/>
       <c r="C17" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="23"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="14"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="25"/>
     </row>
     <row r="18" spans="1:13" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="17"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="29" t="s">
+      <c r="E18" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="11"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="I18" s="30"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="L18" s="11"/>
-      <c r="M18" s="12"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="L18" s="29"/>
+      <c r="M18" s="30"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="17"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="23"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="14"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="25"/>
     </row>
     <row r="20" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
-      <c r="B20" s="17"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="37"/>
       <c r="C20" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="29" t="s">
+      <c r="E20" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="11"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="I20" s="30"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="L20" s="9"/>
-      <c r="M20" s="10"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" s="16"/>
+      <c r="M20" s="17"/>
     </row>
     <row r="21" spans="1:13" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
-      <c r="B21" s="17"/>
+      <c r="A21" s="36"/>
+      <c r="B21" s="37"/>
       <c r="C21" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="44"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="46" t="s">
+      <c r="E21" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="39"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="I21" s="47"/>
-      <c r="J21" s="48"/>
-      <c r="K21" s="38" t="s">
+      <c r="I21" s="42"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="L21" s="38"/>
-      <c r="M21" s="39"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="48"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
-      <c r="B22" s="17"/>
+      <c r="A22" s="36"/>
+      <c r="B22" s="37"/>
       <c r="C22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="23"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="14"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
+      <c r="E22" s="18"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="25"/>
+    </row>
+    <row r="23" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="17"/>
+      <c r="B23" s="37"/>
       <c r="C23" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" s="24"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="I23" s="33"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L23" s="13"/>
-      <c r="M23" s="14"/>
+      <c r="E23" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="32"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="L23" s="16"/>
+      <c r="M23" s="17"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="17"/>
+      <c r="A24" s="36"/>
+      <c r="B24" s="37"/>
       <c r="C24" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="23"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="14"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="25"/>
     </row>
     <row r="25" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="17"/>
+      <c r="A25" s="36"/>
+      <c r="B25" s="37"/>
       <c r="C25" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="40" t="s">
+      <c r="E25" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="41"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="29" t="s">
+      <c r="F25" s="45"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="I25" s="30"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="L25" s="9"/>
-      <c r="M25" s="10"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="L25" s="16"/>
+      <c r="M25" s="17"/>
     </row>
     <row r="26" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
-      <c r="B26" s="17"/>
+      <c r="A26" s="36"/>
+      <c r="B26" s="37"/>
       <c r="C26" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="20" t="s">
+      <c r="E26" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" s="36"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="L26" s="9"/>
-      <c r="M26" s="10"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" s="32"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="L26" s="16"/>
+      <c r="M26" s="17"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="17"/>
+      <c r="A27" s="36"/>
+      <c r="B27" s="37"/>
       <c r="C27" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E27" s="23"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="10"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
+      <c r="E27" s="18"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="17"/>
+    </row>
+    <row r="28" spans="1:13" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="17"/>
+      <c r="B28" s="37"/>
       <c r="C28" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="F28" s="24"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="32" t="s">
+      <c r="E28" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="11"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="I28" s="33"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L28" s="13"/>
-      <c r="M28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="L28" s="16"/>
+      <c r="M28" s="17"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="17"/>
+      <c r="A29" s="36"/>
+      <c r="B29" s="37"/>
       <c r="C29" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="23"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="34"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="14"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="25"/>
     </row>
     <row r="30" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="17"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="37"/>
       <c r="C30" s="3" t="s">
         <v>19</v>
       </c>
@@ -1474,135 +1480,135 @@
       </c>
       <c r="F30" s="27"/>
       <c r="G30" s="28"/>
-      <c r="H30" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="I30" s="36"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="L30" s="9"/>
-      <c r="M30" s="10"/>
+      <c r="H30" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="I30" s="32"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="L30" s="16"/>
+      <c r="M30" s="17"/>
     </row>
     <row r="31" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
-      <c r="B31" s="17"/>
+      <c r="A31" s="36"/>
+      <c r="B31" s="37"/>
       <c r="C31" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E31" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="F31" s="21"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="29" t="s">
+      <c r="E31" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" s="11"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="I31" s="30"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="9" t="s">
+      <c r="I31" s="14"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="L31" s="9"/>
-      <c r="M31" s="10"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="17"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
-      <c r="B32" s="17"/>
+      <c r="A32" s="36"/>
+      <c r="B32" s="37"/>
       <c r="C32" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E32" s="23"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="14"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="25"/>
     </row>
     <row r="33" spans="1:13" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
+      <c r="A33" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="17"/>
+      <c r="B33" s="37"/>
       <c r="C33" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="F33" s="21"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="I33" s="30"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="L33" s="9"/>
-      <c r="M33" s="10"/>
+      <c r="E33" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" s="11"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I33" s="14"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="L33" s="16"/>
+      <c r="M33" s="17"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
-      <c r="B34" s="17"/>
+      <c r="A34" s="36"/>
+      <c r="B34" s="37"/>
       <c r="C34" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E34" s="23"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="32"/>
-      <c r="I34" s="33"/>
-      <c r="J34" s="34"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="14"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="24"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="25"/>
     </row>
     <row r="35" spans="1:13" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
-      <c r="B35" s="17"/>
+      <c r="A35" s="36"/>
+      <c r="B35" s="37"/>
       <c r="C35" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E35" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="F35" s="21"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="I35" s="30"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="9" t="s">
+      <c r="E35" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F35" s="11"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I35" s="14"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="L35" s="9"/>
-      <c r="M35" s="10"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="17"/>
     </row>
     <row r="36" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="16"/>
-      <c r="B36" s="17"/>
+      <c r="A36" s="36"/>
+      <c r="B36" s="37"/>
       <c r="C36" s="7" t="s">
         <v>4</v>
       </c>
@@ -1614,98 +1620,104 @@
       </c>
       <c r="F36" s="27"/>
       <c r="G36" s="28"/>
-      <c r="H36" s="35" t="s">
+      <c r="H36" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="I36" s="36"/>
-      <c r="J36" s="37"/>
-      <c r="K36" s="11" t="s">
+      <c r="I36" s="32"/>
+      <c r="J36" s="33"/>
+      <c r="K36" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="L36" s="11"/>
-      <c r="M36" s="12"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="30"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="16"/>
-      <c r="B37" s="17"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="37"/>
       <c r="C37" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="37"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="14"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" s="49"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="32"/>
+      <c r="J37" s="33"/>
+      <c r="K37" s="24"/>
+      <c r="L37" s="24"/>
+      <c r="M37" s="25"/>
+    </row>
+    <row r="38" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="9"/>
       <c r="C38" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="20"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="31"/>
-      <c r="K38" s="9"/>
-      <c r="L38" s="9"/>
-      <c r="M38" s="10"/>
+      <c r="E38" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F38" s="11"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I38" s="14"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="L38" s="16"/>
+      <c r="M38" s="17"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="49"/>
-      <c r="B39" s="49"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
       <c r="C39" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E39" s="23"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="33"/>
-      <c r="J39" s="34"/>
-      <c r="K39" s="13"/>
-      <c r="L39" s="13"/>
-      <c r="M39" s="14"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="22"/>
+      <c r="J39" s="23"/>
+      <c r="K39" s="24"/>
+      <c r="L39" s="24"/>
+      <c r="M39" s="25"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="49"/>
-      <c r="B40" s="49"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
       <c r="C40" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E40" s="20"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="30"/>
-      <c r="J40" s="31"/>
-      <c r="K40" s="9"/>
-      <c r="L40" s="9"/>
-      <c r="M40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="17"/>
     </row>
     <row r="41" spans="1:13" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="49"/>
-      <c r="B41" s="49"/>
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
       <c r="C41" s="7" t="s">
         <v>4</v>
       </c>
@@ -1717,133 +1729,38 @@
       </c>
       <c r="F41" s="27"/>
       <c r="G41" s="28"/>
-      <c r="H41" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="I41" s="30"/>
-      <c r="J41" s="31"/>
-      <c r="K41" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="L41" s="11"/>
-      <c r="M41" s="12"/>
+      <c r="H41" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I41" s="14"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="L41" s="29"/>
+      <c r="M41" s="30"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="49"/>
-      <c r="B42" s="49"/>
+      <c r="A42" s="9"/>
+      <c r="B42" s="9"/>
       <c r="C42" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E42" s="23"/>
-      <c r="F42" s="24"/>
-      <c r="G42" s="25"/>
-      <c r="H42" s="35"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="37"/>
-      <c r="K42" s="13"/>
-      <c r="L42" s="13"/>
-      <c r="M42" s="14"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="31"/>
+      <c r="I42" s="32"/>
+      <c r="J42" s="33"/>
+      <c r="K42" s="24"/>
+      <c r="L42" s="24"/>
+      <c r="M42" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="119">
-    <mergeCell ref="A38:B42"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="H38:J38"/>
-    <mergeCell ref="K38:M38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="K39:M39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="K40:M40"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:J41"/>
-    <mergeCell ref="K41:M41"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="K42:M42"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="A5:B7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="E5:G7"/>
-    <mergeCell ref="H5:J7"/>
-    <mergeCell ref="K5:M7"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="A8:B12"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="A13:B17"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="A18:B22"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="A23:B27"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="H25:J25"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="H28:J28"/>
-    <mergeCell ref="H29:J29"/>
-    <mergeCell ref="H30:J30"/>
-    <mergeCell ref="H31:J31"/>
-    <mergeCell ref="H32:J32"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="K28:M28"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="K30:M30"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
     <mergeCell ref="K35:M35"/>
     <mergeCell ref="K36:M36"/>
     <mergeCell ref="K37:M37"/>
@@ -1868,6 +1785,101 @@
     <mergeCell ref="K27:M27"/>
     <mergeCell ref="A28:B32"/>
     <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="H32:J32"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="A23:B27"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="A18:B22"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="A13:B17"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="A5:B7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="E5:G7"/>
+    <mergeCell ref="H5:J7"/>
+    <mergeCell ref="K5:M7"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="A8:B12"/>
+    <mergeCell ref="A38:B42"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:J38"/>
+    <mergeCell ref="K38:M38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="K39:M39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="K40:M40"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:J41"/>
+    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="K42:M42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>